<commit_message>
Chair, Cochair, new platinum partner page
</commit_message>
<xml_diff>
--- a/polls/IROS20_Partners.xlsx
+++ b/polls/IROS20_Partners.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akdba\Desktop\mysite\polls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C87F76-D6DE-49DB-ACF6-E8D1277258D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA41C6CB-4239-40A1-830D-77A5BED988BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{99C90C33-A2F8-49BC-95C2-22A337B4C8DB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{99C90C33-A2F8-49BC-95C2-22A337B4C8DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="301">
   <si>
     <t>Cartegory</t>
   </si>
@@ -723,9 +723,6 @@
     <t>Tactile Sensing II</t>
   </si>
   <si>
-    <t>Brain-Machine interfaces for Human Robot Interaction</t>
-  </si>
-  <si>
     <t>Cognitive Human Robot Interaction</t>
   </si>
   <si>
@@ -888,9 +885,6 @@
     <t>mp4</t>
   </si>
   <si>
-    <t>YouTube</t>
-  </si>
-  <si>
     <t>main</t>
   </si>
   <si>
@@ -903,9 +897,6 @@
     <t>Webpage Link</t>
   </si>
   <si>
-    <t>Samsung</t>
-  </si>
-  <si>
     <t>3D Model Learning</t>
   </si>
   <si>
@@ -930,7 +921,25 @@
     <t>Perception, Action, and Cognition</t>
   </si>
   <si>
-    <t>Naver Labs</t>
+    <t>NAVER LABS</t>
+  </si>
+  <si>
+    <t>Brain-Machine Interfaces for Human Robot Interaction</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Robotis</t>
+  </si>
+  <si>
+    <t>Intuitive</t>
+  </si>
+  <si>
+    <t>mylist</t>
+  </si>
+  <si>
+    <t>SAMSUNG</t>
   </si>
 </sst>
 </file>
@@ -1338,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE3CA7B-2F7F-49E8-81CC-0A8442F28240}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26:F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1369,19 +1378,19 @@
         <v>7</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1392,13 +1401,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F2" s="1">
         <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1406,16 +1415,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F3" s="1">
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1423,16 +1432,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F4" s="1">
         <v>4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1440,22 +1449,22 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>93</v>
       </c>
       <c r="D5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1463,22 +1472,22 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1486,22 +1495,22 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D7" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1509,22 +1518,22 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1532,22 +1541,22 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>99</v>
       </c>
       <c r="D9" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1555,22 +1564,22 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D10" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1578,22 +1587,22 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1601,22 +1610,22 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D12" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1624,22 +1633,22 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>102</v>
       </c>
       <c r="D13" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1647,22 +1656,22 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>103</v>
       </c>
       <c r="D14" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1670,22 +1679,22 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>105</v>
       </c>
       <c r="D15" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1693,22 +1702,22 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>108</v>
       </c>
       <c r="D16" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1716,22 +1725,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>109</v>
       </c>
       <c r="D17" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1739,22 +1748,22 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>110</v>
       </c>
       <c r="D18" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1762,22 +1771,22 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>111</v>
       </c>
       <c r="D19" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1785,22 +1794,22 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>112</v>
       </c>
       <c r="D20" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1808,22 +1817,22 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D21" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1831,22 +1840,22 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D22" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1854,22 +1863,22 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>119</v>
       </c>
       <c r="D23" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1877,22 +1886,22 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>120</v>
       </c>
       <c r="D24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1900,22 +1909,22 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>121</v>
       </c>
       <c r="D25" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1923,25 +1932,25 @@
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="D26" t="s">
+        <v>293</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="D26" t="s">
-        <v>296</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>291</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1949,25 +1958,25 @@
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>179</v>
       </c>
       <c r="D27" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1975,25 +1984,25 @@
         <v>2</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>180</v>
       </c>
       <c r="D28" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2001,25 +2010,25 @@
         <v>2</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>181</v>
       </c>
       <c r="D29" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2027,25 +2036,25 @@
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>191</v>
       </c>
       <c r="D30" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2053,25 +2062,25 @@
         <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>192</v>
       </c>
       <c r="D31" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2079,25 +2088,25 @@
         <v>2</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>193</v>
       </c>
       <c r="D32" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2105,25 +2114,25 @@
         <v>2</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>196</v>
       </c>
       <c r="D33" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2131,25 +2140,25 @@
         <v>2</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D34" t="s">
+        <v>293</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="D34" t="s">
-        <v>296</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>291</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2157,25 +2166,25 @@
         <v>2</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>199</v>
       </c>
       <c r="D35" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2183,25 +2192,25 @@
         <v>2</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>200</v>
       </c>
       <c r="D36" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2209,25 +2218,25 @@
         <v>2</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>201</v>
       </c>
       <c r="D37" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2235,25 +2244,25 @@
         <v>2</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>202</v>
       </c>
       <c r="D38" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2261,25 +2270,25 @@
         <v>2</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>203</v>
       </c>
       <c r="D39" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2287,25 +2296,25 @@
         <v>2</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>204</v>
       </c>
       <c r="D40" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2313,25 +2322,25 @@
         <v>2</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>205</v>
       </c>
       <c r="D41" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2339,25 +2348,25 @@
         <v>2</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>206</v>
       </c>
       <c r="D42" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2365,25 +2374,25 @@
         <v>2</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>177</v>
       </c>
       <c r="D43" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2391,32 +2400,62 @@
         <v>2</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>178</v>
       </c>
       <c r="D44" t="s">
+        <v>293</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="B45" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>299</v>
+      </c>
       <c r="E45" s="3"/>
+      <c r="F45" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="46" spans="1:8">
+      <c r="A46" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>299</v>
+      </c>
       <c r="E46" s="3"/>
+      <c r="F46" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="47" spans="1:8">
       <c r="E47" s="3"/>
@@ -2449,11 +2488,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC02C559-417D-440E-80D7-0AF2D68A3729}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:C260"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="G223" sqref="G223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2474,7 +2512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2485,7 +2523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2496,7 +2534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2507,7 +2545,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2518,7 +2556,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1">
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2526,10 +2564,10 @@
         <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" hidden="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2537,10 +2575,10 @@
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" hidden="1">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2548,10 +2586,10 @@
         <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" hidden="1">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2562,7 +2600,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1">
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2573,7 +2611,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1">
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2584,7 +2622,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" hidden="1">
+    <row r="12" spans="1:3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2595,7 +2633,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3" hidden="1">
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2606,7 +2644,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1">
+    <row r="14" spans="1:3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2617,7 +2655,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1">
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2628,7 +2666,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1">
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2639,7 +2677,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1">
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2650,7 +2688,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:3" hidden="1">
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2661,7 +2699,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1">
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2672,7 +2710,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:3" hidden="1">
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2683,7 +2721,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1">
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2694,7 +2732,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1">
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2705,7 +2743,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:3" hidden="1">
+    <row r="23" spans="1:3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2716,7 +2754,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1">
+    <row r="24" spans="1:3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2727,7 +2765,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1">
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2738,7 +2776,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1">
+    <row r="26" spans="1:3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2749,7 +2787,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" hidden="1">
+    <row r="27" spans="1:3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2757,10 +2795,10 @@
         <v>15</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" hidden="1">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2768,10 +2806,10 @@
         <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" hidden="1">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2782,7 +2820,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:3" hidden="1">
+    <row r="30" spans="1:3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2793,7 +2831,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3" hidden="1">
+    <row r="31" spans="1:3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2804,7 +2842,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3" hidden="1">
+    <row r="32" spans="1:3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2815,7 +2853,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1">
+    <row r="33" spans="1:3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2826,7 +2864,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1">
+    <row r="34" spans="1:3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2837,7 +2875,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1">
+    <row r="35" spans="1:3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2848,7 +2886,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1">
+    <row r="36" spans="1:3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2859,7 +2897,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1">
+    <row r="37" spans="1:3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2870,7 +2908,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1">
+    <row r="38" spans="1:3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2881,7 +2919,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1">
+    <row r="39" spans="1:3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2892,7 +2930,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1">
+    <row r="40" spans="1:3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2903,7 +2941,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1">
+    <row r="41" spans="1:3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2914,7 +2952,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1">
+    <row r="42" spans="1:3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2925,7 +2963,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1">
+    <row r="43" spans="1:3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2936,7 +2974,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:3" hidden="1">
+    <row r="44" spans="1:3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2947,7 +2985,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="1:3" hidden="1">
+    <row r="45" spans="1:3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2958,7 +2996,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1">
+    <row r="46" spans="1:3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2969,7 +3007,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:3" hidden="1">
+    <row r="47" spans="1:3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2980,7 +3018,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:3" hidden="1">
+    <row r="48" spans="1:3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2991,7 +3029,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:3" hidden="1">
+    <row r="49" spans="1:3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3002,7 +3040,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:3" hidden="1">
+    <row r="50" spans="1:3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3013,7 +3051,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:3" hidden="1">
+    <row r="51" spans="1:3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3024,7 +3062,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:3" hidden="1">
+    <row r="52" spans="1:3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3035,7 +3073,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:3" hidden="1">
+    <row r="53" spans="1:3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3046,7 +3084,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:3" hidden="1">
+    <row r="54" spans="1:3">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3057,7 +3095,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:3" hidden="1">
+    <row r="55" spans="1:3">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3068,7 +3106,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:3" hidden="1">
+    <row r="56" spans="1:3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3079,7 +3117,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:3" hidden="1">
+    <row r="57" spans="1:3">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3090,7 +3128,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="58" spans="1:3" hidden="1">
+    <row r="58" spans="1:3">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3101,7 +3139,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="59" spans="1:3" hidden="1">
+    <row r="59" spans="1:3">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3112,7 +3150,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:3" hidden="1">
+    <row r="60" spans="1:3">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3123,7 +3161,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:3" hidden="1">
+    <row r="61" spans="1:3">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3134,7 +3172,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:3" hidden="1">
+    <row r="62" spans="1:3">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -3145,7 +3183,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="63" spans="1:3" hidden="1">
+    <row r="63" spans="1:3">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3156,7 +3194,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:3" hidden="1">
+    <row r="64" spans="1:3">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -3167,7 +3205,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1">
+    <row r="65" spans="1:3">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -3178,7 +3216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:3" hidden="1">
+    <row r="66" spans="1:3">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -3189,7 +3227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1">
+    <row r="67" spans="1:3">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -3200,7 +3238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1">
+    <row r="68" spans="1:3">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -3211,7 +3249,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1">
+    <row r="69" spans="1:3">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -3222,7 +3260,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1">
+    <row r="70" spans="1:3">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -3233,7 +3271,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1">
+    <row r="71" spans="1:3">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -3244,7 +3282,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1">
+    <row r="72" spans="1:3">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -3255,7 +3293,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1">
+    <row r="73" spans="1:3">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -3266,7 +3304,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1">
+    <row r="74" spans="1:3">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3277,7 +3315,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1">
+    <row r="75" spans="1:3">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -3288,7 +3326,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1">
+    <row r="76" spans="1:3">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -3307,7 +3345,7 @@
         <v>18</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -3417,7 +3455,7 @@
         <v>18</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -3428,7 +3466,7 @@
         <v>18</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -3439,7 +3477,7 @@
         <v>18</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -3582,7 +3620,7 @@
         <v>18</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -3593,7 +3631,7 @@
         <v>18</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -3761,7 +3799,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="119" spans="1:3" hidden="1">
+    <row r="119" spans="1:3">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -3772,7 +3810,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="120" spans="1:3" hidden="1">
+    <row r="120" spans="1:3">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -3783,7 +3821,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="121" spans="1:3" hidden="1">
+    <row r="121" spans="1:3">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -3794,7 +3832,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="122" spans="1:3" hidden="1">
+    <row r="122" spans="1:3">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -3805,7 +3843,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="123" spans="1:3" hidden="1">
+    <row r="123" spans="1:3">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -3816,7 +3854,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="124" spans="1:3" hidden="1">
+    <row r="124" spans="1:3">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -3827,7 +3865,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="125" spans="1:3" hidden="1">
+    <row r="125" spans="1:3">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -3838,7 +3876,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="126" spans="1:3" hidden="1">
+    <row r="126" spans="1:3">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -3849,7 +3887,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="127" spans="1:3" hidden="1">
+    <row r="127" spans="1:3">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -3860,7 +3898,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="128" spans="1:3" hidden="1">
+    <row r="128" spans="1:3">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -3871,7 +3909,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="129" spans="1:3" hidden="1">
+    <row r="129" spans="1:3">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -3882,7 +3920,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="130" spans="1:3" hidden="1">
+    <row r="130" spans="1:3">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -3893,7 +3931,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="131" spans="1:3" hidden="1">
+    <row r="131" spans="1:3">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -3904,7 +3942,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="132" spans="1:3" hidden="1">
+    <row r="132" spans="1:3">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -3915,7 +3953,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="133" spans="1:3" hidden="1">
+    <row r="133" spans="1:3">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -3926,7 +3964,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="134" spans="1:3" hidden="1">
+    <row r="134" spans="1:3">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -3937,7 +3975,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="135" spans="1:3" hidden="1">
+    <row r="135" spans="1:3">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -3948,7 +3986,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="136" spans="1:3" hidden="1">
+    <row r="136" spans="1:3">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -3959,7 +3997,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="137" spans="1:3" hidden="1">
+    <row r="137" spans="1:3">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -3970,7 +4008,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="138" spans="1:3" hidden="1">
+    <row r="138" spans="1:3">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -3981,7 +4019,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="139" spans="1:3" hidden="1">
+    <row r="139" spans="1:3">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -3992,7 +4030,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="140" spans="1:3" hidden="1">
+    <row r="140" spans="1:3">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -4003,7 +4041,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="141" spans="1:3" hidden="1">
+    <row r="141" spans="1:3">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -4014,7 +4052,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="142" spans="1:3" hidden="1">
+    <row r="142" spans="1:3">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -4025,7 +4063,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="143" spans="1:3" hidden="1">
+    <row r="143" spans="1:3">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -4036,7 +4074,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="144" spans="1:3" hidden="1">
+    <row r="144" spans="1:3">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -4047,7 +4085,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="145" spans="1:3" hidden="1">
+    <row r="145" spans="1:3">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -4058,7 +4096,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="146" spans="1:3" hidden="1">
+    <row r="146" spans="1:3">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -4066,10 +4104,10 @@
         <v>20</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" hidden="1">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -4077,10 +4115,10 @@
         <v>20</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" hidden="1">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -4091,7 +4129,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="149" spans="1:3" hidden="1">
+    <row r="149" spans="1:3">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -4102,7 +4140,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="150" spans="1:3" hidden="1">
+    <row r="150" spans="1:3">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -4113,7 +4151,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="151" spans="1:3" hidden="1">
+    <row r="151" spans="1:3">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -4121,10 +4159,10 @@
         <v>20</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" hidden="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -4135,7 +4173,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="153" spans="1:3" hidden="1">
+    <row r="153" spans="1:3">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -4146,7 +4184,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="154" spans="1:3" hidden="1">
+    <row r="154" spans="1:3">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -4157,7 +4195,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="155" spans="1:3" hidden="1">
+    <row r="155" spans="1:3">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -4168,7 +4206,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="156" spans="1:3" hidden="1">
+    <row r="156" spans="1:3">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -4179,7 +4217,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="157" spans="1:3" hidden="1">
+    <row r="157" spans="1:3">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -4190,7 +4228,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="158" spans="1:3" hidden="1">
+    <row r="158" spans="1:3">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -4201,7 +4239,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="159" spans="1:3" hidden="1">
+    <row r="159" spans="1:3">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -4212,7 +4250,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="160" spans="1:3" hidden="1">
+    <row r="160" spans="1:3">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -4223,7 +4261,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="161" spans="1:3" hidden="1">
+    <row r="161" spans="1:3">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -4234,7 +4272,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="162" spans="1:3" hidden="1">
+    <row r="162" spans="1:3">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -4245,7 +4283,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="163" spans="1:3" hidden="1">
+    <row r="163" spans="1:3">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -4256,7 +4294,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="164" spans="1:3" hidden="1">
+    <row r="164" spans="1:3">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -4267,7 +4305,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="165" spans="1:3" hidden="1">
+    <row r="165" spans="1:3">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -4278,7 +4316,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="166" spans="1:3" hidden="1">
+    <row r="166" spans="1:3">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -4286,10 +4324,10 @@
         <v>20</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" hidden="1">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -4300,7 +4338,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="168" spans="1:3" hidden="1">
+    <row r="168" spans="1:3">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -4311,7 +4349,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="169" spans="1:3" hidden="1">
+    <row r="169" spans="1:3">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -4322,7 +4360,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="170" spans="1:3" hidden="1">
+    <row r="170" spans="1:3">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -4333,7 +4371,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="171" spans="1:3" hidden="1">
+    <row r="171" spans="1:3">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -4344,7 +4382,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="172" spans="1:3" hidden="1">
+    <row r="172" spans="1:3">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -4355,7 +4393,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="173" spans="1:3" hidden="1">
+    <row r="173" spans="1:3">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -4366,7 +4404,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="174" spans="1:3" hidden="1">
+    <row r="174" spans="1:3">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -4377,7 +4415,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="175" spans="1:3" hidden="1">
+    <row r="175" spans="1:3">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -4388,7 +4426,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="176" spans="1:3" hidden="1">
+    <row r="176" spans="1:3">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -4399,7 +4437,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="177" spans="1:3" hidden="1">
+    <row r="177" spans="1:3">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -4410,7 +4448,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="178" spans="1:3" hidden="1">
+    <row r="178" spans="1:3">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -4421,7 +4459,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="179" spans="1:3" hidden="1">
+    <row r="179" spans="1:3">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -4432,7 +4470,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="180" spans="1:3" hidden="1">
+    <row r="180" spans="1:3">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -4443,7 +4481,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="181" spans="1:3" hidden="1">
+    <row r="181" spans="1:3">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -4454,7 +4492,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="182" spans="1:3" hidden="1">
+    <row r="182" spans="1:3">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -4465,7 +4503,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="183" spans="1:3" hidden="1">
+    <row r="183" spans="1:3">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -4476,7 +4514,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="184" spans="1:3" hidden="1">
+    <row r="184" spans="1:3">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -4487,7 +4525,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="185" spans="1:3" hidden="1">
+    <row r="185" spans="1:3">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -4498,7 +4536,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="186" spans="1:3" hidden="1">
+    <row r="186" spans="1:3">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -4509,7 +4547,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="187" spans="1:3" hidden="1">
+    <row r="187" spans="1:3">
       <c r="A187" s="1">
         <v>186</v>
       </c>
@@ -4520,7 +4558,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="188" spans="1:3" hidden="1">
+    <row r="188" spans="1:3">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -4531,7 +4569,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="189" spans="1:3" hidden="1">
+    <row r="189" spans="1:3">
       <c r="A189" s="1">
         <v>188</v>
       </c>
@@ -4542,7 +4580,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="190" spans="1:3" hidden="1">
+    <row r="190" spans="1:3">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -4553,7 +4591,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="191" spans="1:3" hidden="1">
+    <row r="191" spans="1:3">
       <c r="A191" s="1">
         <v>190</v>
       </c>
@@ -4564,7 +4602,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="192" spans="1:3" hidden="1">
+    <row r="192" spans="1:3">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -4575,7 +4613,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="193" spans="1:3" hidden="1">
+    <row r="193" spans="1:3">
       <c r="A193" s="1">
         <v>192</v>
       </c>
@@ -4586,7 +4624,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="194" spans="1:3" hidden="1">
+    <row r="194" spans="1:3">
       <c r="A194" s="1">
         <v>193</v>
       </c>
@@ -4597,7 +4635,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="195" spans="1:3" hidden="1">
+    <row r="195" spans="1:3">
       <c r="A195" s="1">
         <v>194</v>
       </c>
@@ -4608,7 +4646,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="196" spans="1:3" hidden="1">
+    <row r="196" spans="1:3">
       <c r="A196" s="1">
         <v>195</v>
       </c>
@@ -4619,7 +4657,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="197" spans="1:3" hidden="1">
+    <row r="197" spans="1:3">
       <c r="A197" s="1">
         <v>196</v>
       </c>
@@ -4630,7 +4668,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="198" spans="1:3" hidden="1">
+    <row r="198" spans="1:3">
       <c r="A198" s="1">
         <v>197</v>
       </c>
@@ -4641,7 +4679,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="199" spans="1:3" hidden="1">
+    <row r="199" spans="1:3">
       <c r="A199" s="1">
         <v>198</v>
       </c>
@@ -4652,7 +4690,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="200" spans="1:3" hidden="1">
+    <row r="200" spans="1:3">
       <c r="A200" s="1">
         <v>199</v>
       </c>
@@ -4663,7 +4701,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="201" spans="1:3" hidden="1">
+    <row r="201" spans="1:3">
       <c r="A201" s="1">
         <v>200</v>
       </c>
@@ -4674,7 +4712,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="202" spans="1:3" hidden="1">
+    <row r="202" spans="1:3">
       <c r="A202" s="1">
         <v>201</v>
       </c>
@@ -4685,7 +4723,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="203" spans="1:3" hidden="1">
+    <row r="203" spans="1:3">
       <c r="A203" s="1">
         <v>202</v>
       </c>
@@ -4696,7 +4734,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="204" spans="1:3" hidden="1">
+    <row r="204" spans="1:3">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -4707,7 +4745,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="205" spans="1:3" hidden="1">
+    <row r="205" spans="1:3">
       <c r="A205" s="1">
         <v>204</v>
       </c>
@@ -4718,7 +4756,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="206" spans="1:3" hidden="1">
+    <row r="206" spans="1:3">
       <c r="A206" s="1">
         <v>205</v>
       </c>
@@ -4729,7 +4767,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="207" spans="1:3" hidden="1">
+    <row r="207" spans="1:3">
       <c r="A207" s="1">
         <v>206</v>
       </c>
@@ -4740,7 +4778,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="208" spans="1:3" hidden="1">
+    <row r="208" spans="1:3">
       <c r="A208" s="1">
         <v>207</v>
       </c>
@@ -4751,7 +4789,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="209" spans="1:3" hidden="1">
+    <row r="209" spans="1:3">
       <c r="A209" s="1">
         <v>208</v>
       </c>
@@ -4762,7 +4800,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="210" spans="1:3" hidden="1">
+    <row r="210" spans="1:3">
       <c r="A210" s="1">
         <v>209</v>
       </c>
@@ -4773,7 +4811,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="211" spans="1:3" hidden="1">
+    <row r="211" spans="1:3">
       <c r="A211" s="1">
         <v>210</v>
       </c>
@@ -4784,7 +4822,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="212" spans="1:3" hidden="1">
+    <row r="212" spans="1:3">
       <c r="A212" s="1">
         <v>211</v>
       </c>
@@ -4795,7 +4833,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="213" spans="1:3" hidden="1">
+    <row r="213" spans="1:3">
       <c r="A213" s="1">
         <v>212</v>
       </c>
@@ -4806,7 +4844,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="214" spans="1:3" hidden="1">
+    <row r="214" spans="1:3">
       <c r="A214" s="1">
         <v>213</v>
       </c>
@@ -4817,7 +4855,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="215" spans="1:3" hidden="1">
+    <row r="215" spans="1:3">
       <c r="A215" s="1">
         <v>214</v>
       </c>
@@ -4828,7 +4866,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="216" spans="1:3" hidden="1">
+    <row r="216" spans="1:3">
       <c r="A216" s="1">
         <v>215</v>
       </c>
@@ -4839,7 +4877,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="217" spans="1:3" hidden="1">
+    <row r="217" spans="1:3">
       <c r="A217" s="1">
         <v>216</v>
       </c>
@@ -4847,10 +4885,10 @@
         <v>21</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" hidden="1">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
       <c r="A218" s="1">
         <v>217</v>
       </c>
@@ -4858,10 +4896,10 @@
         <v>21</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" hidden="1">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
       <c r="A219" s="1">
         <v>218</v>
       </c>
@@ -4872,7 +4910,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="220" spans="1:3" hidden="1">
+    <row r="220" spans="1:3">
       <c r="A220" s="1">
         <v>219</v>
       </c>
@@ -4883,7 +4921,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="221" spans="1:3" hidden="1">
+    <row r="221" spans="1:3">
       <c r="A221" s="1">
         <v>220</v>
       </c>
@@ -4894,7 +4932,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="222" spans="1:3" hidden="1">
+    <row r="222" spans="1:3">
       <c r="A222" s="1">
         <v>221</v>
       </c>
@@ -4905,7 +4943,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="223" spans="1:3" hidden="1">
+    <row r="223" spans="1:3">
       <c r="A223" s="1">
         <v>222</v>
       </c>
@@ -4916,7 +4954,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="224" spans="1:3" hidden="1">
+    <row r="224" spans="1:3">
       <c r="A224" s="1">
         <v>223</v>
       </c>
@@ -4924,10 +4962,10 @@
         <v>21</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" hidden="1">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
       <c r="A225" s="1">
         <v>224</v>
       </c>
@@ -4935,10 +4973,10 @@
         <v>23</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" hidden="1">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
       <c r="A226" s="1">
         <v>225</v>
       </c>
@@ -4946,10 +4984,10 @@
         <v>23</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" hidden="1">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3">
       <c r="A227" s="1">
         <v>226</v>
       </c>
@@ -4957,10 +4995,10 @@
         <v>23</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" hidden="1">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
       <c r="A228" s="1">
         <v>227</v>
       </c>
@@ -4968,10 +5006,10 @@
         <v>23</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" hidden="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
       <c r="A229" s="1">
         <v>228</v>
       </c>
@@ -4979,10 +5017,10 @@
         <v>23</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" hidden="1">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
       <c r="A230" s="1">
         <v>229</v>
       </c>
@@ -4990,10 +5028,10 @@
         <v>23</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" hidden="1">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
       <c r="A231" s="1">
         <v>230</v>
       </c>
@@ -5001,10 +5039,10 @@
         <v>23</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" hidden="1">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
       <c r="A232" s="1">
         <v>231</v>
       </c>
@@ -5012,10 +5050,10 @@
         <v>23</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3" hidden="1">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
       <c r="A233" s="1">
         <v>232</v>
       </c>
@@ -5023,10 +5061,10 @@
         <v>23</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" hidden="1">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
       <c r="A234" s="1">
         <v>233</v>
       </c>
@@ -5034,10 +5072,10 @@
         <v>23</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" hidden="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
       <c r="A235" s="1">
         <v>234</v>
       </c>
@@ -5045,10 +5083,10 @@
         <v>23</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" hidden="1">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
       <c r="A236" s="1">
         <v>235</v>
       </c>
@@ -5056,10 +5094,10 @@
         <v>23</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" hidden="1">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3">
       <c r="A237" s="1">
         <v>236</v>
       </c>
@@ -5067,10 +5105,10 @@
         <v>23</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" hidden="1">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
       <c r="A238" s="1">
         <v>237</v>
       </c>
@@ -5078,10 +5116,10 @@
         <v>23</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" hidden="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
       <c r="A239" s="1">
         <v>238</v>
       </c>
@@ -5089,10 +5127,10 @@
         <v>23</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" hidden="1">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
       <c r="A240" s="1">
         <v>239</v>
       </c>
@@ -5100,10 +5138,10 @@
         <v>23</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" hidden="1">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3">
       <c r="A241" s="1">
         <v>240</v>
       </c>
@@ -5111,10 +5149,10 @@
         <v>23</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" hidden="1">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
       <c r="A242" s="1">
         <v>241</v>
       </c>
@@ -5122,10 +5160,10 @@
         <v>24</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" hidden="1">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
       <c r="A243" s="1">
         <v>242</v>
       </c>
@@ -5133,10 +5171,10 @@
         <v>24</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" hidden="1">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3">
       <c r="A244" s="1">
         <v>243</v>
       </c>
@@ -5144,10 +5182,10 @@
         <v>24</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3" hidden="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3">
       <c r="A245" s="1">
         <v>244</v>
       </c>
@@ -5155,10 +5193,10 @@
         <v>24</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3" hidden="1">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
       <c r="A246" s="1">
         <v>245</v>
       </c>
@@ -5166,10 +5204,10 @@
         <v>24</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" hidden="1">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
       <c r="A247" s="1">
         <v>246</v>
       </c>
@@ -5177,10 +5215,10 @@
         <v>24</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3" hidden="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
       <c r="A248" s="1">
         <v>247</v>
       </c>
@@ -5188,10 +5226,10 @@
         <v>24</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" hidden="1">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3">
       <c r="A249" s="1">
         <v>248</v>
       </c>
@@ -5199,10 +5237,10 @@
         <v>24</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3" hidden="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
       <c r="A250" s="1">
         <v>249</v>
       </c>
@@ -5210,10 +5248,10 @@
         <v>24</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3" hidden="1">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
       <c r="A251" s="1">
         <v>250</v>
       </c>
@@ -5221,10 +5259,10 @@
         <v>24</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" hidden="1">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
       <c r="A252" s="1">
         <v>251</v>
       </c>
@@ -5232,10 +5270,10 @@
         <v>24</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" hidden="1">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
       <c r="A253" s="1">
         <v>252</v>
       </c>
@@ -5243,10 +5281,10 @@
         <v>25</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3" hidden="1">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
       <c r="A254" s="1">
         <v>253</v>
       </c>
@@ -5254,10 +5292,10 @@
         <v>25</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3" hidden="1">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
       <c r="A255" s="1">
         <v>254</v>
       </c>
@@ -5265,10 +5303,10 @@
         <v>25</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3" hidden="1">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3">
       <c r="A256" s="1">
         <v>255</v>
       </c>
@@ -5276,10 +5314,10 @@
         <v>25</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3" hidden="1">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
       <c r="A257" s="1">
         <v>256</v>
       </c>
@@ -5287,10 +5325,10 @@
         <v>25</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3" hidden="1">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3">
       <c r="A258" s="1">
         <v>257</v>
       </c>
@@ -5298,10 +5336,10 @@
         <v>25</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3" hidden="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3">
       <c r="A259" s="1">
         <v>258</v>
       </c>
@@ -5309,10 +5347,10 @@
         <v>25</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3" hidden="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3">
       <c r="A260" s="1">
         <v>259</v>
       </c>
@@ -5324,13 +5362,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C260" xr:uid="{1B8703AA-0DCD-40E4-945C-71786370758E}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Localization, Mapping and Navigation "/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C260" xr:uid="{1B8703AA-0DCD-40E4-945C-71786370758E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bug fix since the first day open
</commit_message>
<xml_diff>
--- a/polls/IROS20_Partners.xlsx
+++ b/polls/IROS20_Partners.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akdba\Desktop\mysite\polls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60995A16-C777-4CB8-B948-F1EB6BDD8036}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426D6DA1-0753-4F63-BF0C-78C382F40CEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{99C90C33-A2F8-49BC-95C2-22A337B4C8DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{99C90C33-A2F8-49BC-95C2-22A337B4C8DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="349">
   <si>
     <t>Cartegory</t>
   </si>
@@ -1155,7 +1155,16 @@
     <t>At Amazon we fundamentally believe that scientific innovation is essential to being the most customer-centric company in the world. It's this ability to have an impact at scale that allows us to attract some of the brightest minds in robotics. Come and build the future with us!</t>
   </si>
   <si>
-    <t xml:space="preserve">              </t>
+    <t>NVIDIA is enabling the next generation of Autonomous Machines. From manufacturing, retail, logistics, agriculture, health care and beyond, developers are creating breakthrough Robotics and AI applications on the NVIDIA Jetson platform.</t>
+  </si>
+  <si>
+    <t>EAI Technology</t>
+  </si>
+  <si>
+    <t>EAI Technology is a professional LiDAR sensor brand worldwide. YDLIDAR is committed to LiDAR applications in AI robotics education</t>
+  </si>
+  <si>
+    <t>https://www.ydlidar.com/</t>
   </si>
 </sst>
 </file>
@@ -1786,8 +1795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE3CA7B-2F7F-49E8-81CC-0A8442F28240}">
   <dimension ref="A1:J145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3923,6 +3932,29 @@
         <v>339</v>
       </c>
     </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="1">
+        <v>20017</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
     <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>20004</v>
@@ -5747,10 +5779,11 @@
     <hyperlink ref="F46" r:id="rId16" xr:uid="{B8127B5E-72D6-4430-B840-CF6FECE02181}"/>
     <hyperlink ref="F50" r:id="rId17" xr:uid="{3AAF3E8A-6255-45B0-B677-CA6ABC2BFEEF}"/>
     <hyperlink ref="F49" r:id="rId18" xr:uid="{92F087A9-A4FF-44EE-B0DF-9D977F98B356}"/>
+    <hyperlink ref="F74" r:id="rId19" xr:uid="{49937CE6-E8D5-4157-A59D-3DF456C32564}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
-  <legacyDrawing r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
+  <legacyDrawing r:id="rId21"/>
 </worksheet>
 </file>
 

</xml_diff>